<commit_message>
update(): Button and Excel File
</commit_message>
<xml_diff>
--- a/public/uploads/templates/allowance_templates.xlsx
+++ b/public/uploads/templates/allowance_templates.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gemin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\fp\public\uploads\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283BCB57-65D4-42A4-97A6-133B82D4F1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4A0B58E-2CC3-45B1-A427-ADB61D7F4F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7810" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>payroll number</t>
   </si>
@@ -33,16 +33,19 @@
     <t>Employee Name</t>
   </si>
   <si>
-    <t>Deogratias Mushi</t>
-  </si>
-  <si>
-    <t>TZS</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>xxxxxx</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
+  </si>
+  <si>
+    <t>TZS/ USD</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -501,24 +504,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>100281</v>
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>100000</v>
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>